<commit_message>
Adrien - MAJ Journa de travail
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Adrien/Journal_Travail.xlsx
+++ b/Dossiers personnels/Adrien/Journal_Travail.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="25" documentId="11_F7D032B5AE6E561E8C9E2EE3721ACA7E57B54412" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{DDA1D708-1E8E-46D7-B459-F62FC0D359AC}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="11_F7D032B5AE6E561E8C9E2EE3721ACA7E57B54412" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{C87D5291-EA2B-4425-B822-97727DD90AC7}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
@@ -56,6 +56,24 @@
   </si>
   <si>
     <t>Call pour le cahier des charges</t>
+  </si>
+  <si>
+    <t>Réunion pour définir model</t>
+  </si>
+  <si>
+    <t>Mise en commun et discution avec M.Rentch du cahier des charges</t>
+  </si>
+  <si>
+    <t>16/03/18</t>
+  </si>
+  <si>
+    <t>Discution de groupe du model</t>
+  </si>
+  <si>
+    <t>18/03/18</t>
+  </si>
+  <si>
+    <t>Recherche et test du model conceptuel Commande</t>
   </si>
 </sst>
 </file>
@@ -456,7 +474,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,24 +574,48 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="8"/>
+      <c r="A11" s="3">
+        <v>43168</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>43171</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -671,7 +713,7 @@
       </c>
       <c r="C33" s="9">
         <f>SUM(C5:C32)</f>
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journal de travail updated
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Adrien/Journal_Travail.xlsx
+++ b/Dossiers personnels/Adrien/Journal_Travail.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="71" documentId="11_F7D032B5AE6E561E8C9E2EE3721ACA7E57B54412" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{41A3A0AC-FFA3-472C-AD10-A60BB45088F1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98A0324-30B5-46DC-AC03-CFA8F0DC1CC7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3750" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>Remaniement du modèle MVD, restructuration des dossiers, travail sur le crayon et la gomme et recherches sur la structure "canevas" de FXML</t>
+  </si>
+  <si>
+    <t>Implémentation de l'historique sur les fonctionnalités outils</t>
+  </si>
+  <si>
+    <t>suite de l'implémentation de l'historique</t>
+  </si>
+  <si>
+    <t>finalisation de l'ordre des calques</t>
   </si>
 </sst>
 </file>
@@ -507,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -729,24 +738,44 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
+      <c r="A22" s="3">
+        <v>43195</v>
+      </c>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="8"/>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>43200</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" s="8">
+        <v>13</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="8"/>
+      <c r="A24" s="3">
+        <v>43201</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="8">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="3">
+        <v>43204</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -789,12 +818,17 @@
       <c r="C33" s="8"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" s="5" t="s">
+      <c r="A34" s="3"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C34" s="9">
-        <f>SUM(C5:C33)</f>
-        <v>45</v>
+      <c r="C35" s="9">
+        <f>SUM(C5:C34)</f>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
analyse de la répartition du temps de travail I
</commit_message>
<xml_diff>
--- a/Dossiers personnels/Adrien/Journal_Travail.xlsx
+++ b/Dossiers personnels/Adrien/Journal_Travail.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A58EC11-553B-4B89-97D6-5199A3C3EC9E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9465CF1-E8F3-46C2-AE59-2C2A1F17D016}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4710" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5670" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
   <si>
     <t>Date</t>
   </si>
@@ -124,9 +124,6 @@
     <t>Divers tests d'utilisation</t>
   </si>
   <si>
-    <t>Image d egroupe 1</t>
-  </si>
-  <si>
     <t>18/05/18</t>
   </si>
   <si>
@@ -145,10 +142,7 @@
     <t>Analyse du travail + rapport</t>
   </si>
   <si>
-    <t>21/5/18</t>
-  </si>
-  <si>
-    <t>finalisation du rapport</t>
+    <t>Image de groupe 1</t>
   </si>
 </sst>
 </file>
@@ -546,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,7 +715,9 @@
       <c r="B17" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="8">
+        <v>2</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -809,7 +805,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>33</v>
@@ -820,10 +816,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C27" s="8">
         <v>1</v>
@@ -831,10 +827,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C28" s="8">
         <v>3</v>
@@ -842,25 +838,19 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>39</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>40</v>
       </c>
       <c r="C29" s="8">
         <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C30" s="8">
-        <v>2</v>
-      </c>
+      <c r="A30" s="3"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
@@ -878,16 +868,11 @@
       <c r="C33" s="8"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="8"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B35" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C35" s="9">
-        <f>SUM(C5:C34)</f>
+      <c r="C34" s="9">
+        <f>SUM(C5:C33)</f>
         <v>89</v>
       </c>
     </row>

</xml_diff>